<commit_message>
WHO Sit Rep No 14
</commit_message>
<xml_diff>
--- a/who-confirmed-cases.xlsx
+++ b/who-confirmed-cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mink/Documents/GitHub/NovelCoronavirusData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mink/Documents/GitHub/2019-nCoV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A25743-E868-1849-8132-7B19B7FD1070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C0E877F-1934-6947-9E25-4822C7CD0AE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WHO-Data" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="75">
   <si>
     <t>China</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>NotAvail</t>
+  </si>
+  <si>
+    <t>Cases with Travel history to China</t>
+  </si>
+  <si>
+    <t>Possible Confirmed transmission outside China</t>
+  </si>
+  <si>
+    <t>Transmission Site under investigation</t>
   </si>
 </sst>
 </file>
@@ -1531,10 +1540,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8641C3A-DA45-1B41-BC10-1E7E8EC457C5}">
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D251" sqref="D251"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H275" sqref="H275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1545,7 +1556,7 @@
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="70" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1561,8 +1572,17 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>43850</v>
       </c>
@@ -1579,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>43850</v>
       </c>
@@ -1596,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>43850</v>
       </c>
@@ -1613,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>43850</v>
       </c>
@@ -1630,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>43850</v>
       </c>
@@ -1647,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>43850</v>
       </c>
@@ -1664,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>43850</v>
       </c>
@@ -1681,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>43850</v>
       </c>
@@ -1698,7 +1718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>43852</v>
       </c>
@@ -1715,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>43852</v>
       </c>
@@ -1732,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>43852</v>
       </c>
@@ -1749,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>43852</v>
       </c>
@@ -1766,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>43852</v>
       </c>
@@ -1783,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>43852</v>
       </c>
@@ -1800,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>43852</v>
       </c>
@@ -5609,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A241" s="10">
         <v>43863</v>
       </c>
@@ -5626,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A242" s="10">
         <v>43863</v>
       </c>
@@ -5643,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A243" s="10">
         <v>43863</v>
       </c>
@@ -5660,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A244" s="10">
         <v>43863</v>
       </c>
@@ -5677,7 +5697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A245" s="10">
         <v>43863</v>
       </c>
@@ -5694,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A246" s="10">
         <v>43863</v>
       </c>
@@ -5711,7 +5731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:5" ht="17" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:8" ht="17" x14ac:dyDescent="0.15">
       <c r="A247" s="10">
         <v>43863</v>
       </c>
@@ -5728,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A248" s="10">
         <v>43863</v>
       </c>
@@ -5745,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A249" s="10">
         <v>43863</v>
       </c>
@@ -5762,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A250" s="10">
         <v>43863</v>
       </c>
@@ -5776,6 +5796,672 @@
         <v>10</v>
       </c>
       <c r="E250" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A251" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B251" s="11">
+        <v>14</v>
+      </c>
+      <c r="C251" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D251" s="12">
+        <v>17238</v>
+      </c>
+      <c r="E251" s="12">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A252" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B252" s="11">
+        <v>14</v>
+      </c>
+      <c r="C252" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D252" s="12">
+        <v>20</v>
+      </c>
+      <c r="E252" s="12">
+        <v>0</v>
+      </c>
+      <c r="F252">
+        <v>17</v>
+      </c>
+      <c r="G252">
+        <v>3</v>
+      </c>
+      <c r="H252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A253" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B253" s="11">
+        <v>14</v>
+      </c>
+      <c r="C253" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D253" s="12">
+        <v>15</v>
+      </c>
+      <c r="E253" s="12">
+        <v>0</v>
+      </c>
+      <c r="F253">
+        <v>8</v>
+      </c>
+      <c r="G253">
+        <v>4</v>
+      </c>
+      <c r="H253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A254" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B254" s="11">
+        <v>14</v>
+      </c>
+      <c r="C254" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D254" s="12">
+        <v>8</v>
+      </c>
+      <c r="E254" s="12">
+        <v>0</v>
+      </c>
+      <c r="F254">
+        <v>6</v>
+      </c>
+      <c r="G254">
+        <v>2</v>
+      </c>
+      <c r="H254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A255" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B255" s="11">
+        <v>14</v>
+      </c>
+      <c r="C255" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D255" s="12">
+        <v>18</v>
+      </c>
+      <c r="E255" s="12">
+        <v>0</v>
+      </c>
+      <c r="F255">
+        <v>18</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A256" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B256" s="11">
+        <v>14</v>
+      </c>
+      <c r="C256" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D256" s="12">
+        <v>12</v>
+      </c>
+      <c r="E256" s="12">
+        <v>0</v>
+      </c>
+      <c r="F256">
+        <v>12</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+      <c r="H256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A257" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B257" s="11">
+        <v>14</v>
+      </c>
+      <c r="C257" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D257" s="12">
+        <v>8</v>
+      </c>
+      <c r="E257" s="12">
+        <v>0</v>
+      </c>
+      <c r="F257">
+        <v>7</v>
+      </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
+      <c r="H257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A258" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B258" s="11">
+        <v>14</v>
+      </c>
+      <c r="C258" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D258" s="12">
+        <v>1</v>
+      </c>
+      <c r="E258" s="12">
+        <v>0</v>
+      </c>
+      <c r="F258">
+        <v>1</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A259" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B259" s="11">
+        <v>14</v>
+      </c>
+      <c r="C259" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D259" s="12">
+        <v>2</v>
+      </c>
+      <c r="E259" s="12">
+        <v>1</v>
+      </c>
+      <c r="F259">
+        <v>1</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+      <c r="H259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A260" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B260" s="11">
+        <v>14</v>
+      </c>
+      <c r="C260" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D260" s="12">
+        <v>19</v>
+      </c>
+      <c r="E260" s="12">
+        <v>0</v>
+      </c>
+      <c r="F260">
+        <v>18</v>
+      </c>
+      <c r="G260">
+        <v>1</v>
+      </c>
+      <c r="H260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A261" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B261" s="11">
+        <v>14</v>
+      </c>
+      <c r="C261" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D261" s="12">
+        <v>1</v>
+      </c>
+      <c r="E261" s="12">
+        <v>0</v>
+      </c>
+      <c r="F261">
+        <v>1</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+      <c r="H261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A262" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B262" s="11">
+        <v>14</v>
+      </c>
+      <c r="C262" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D262" s="12">
+        <v>1</v>
+      </c>
+      <c r="E262" s="12">
+        <v>0</v>
+      </c>
+      <c r="F262">
+        <v>1</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+      <c r="H262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A263" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B263" s="11">
+        <v>14</v>
+      </c>
+      <c r="C263" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D263" s="12">
+        <v>3</v>
+      </c>
+      <c r="E263" s="12">
+        <v>0</v>
+      </c>
+      <c r="F263">
+        <v>3</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+      <c r="H263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A264" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B264" s="11">
+        <v>14</v>
+      </c>
+      <c r="C264" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D264" s="12">
+        <v>11</v>
+      </c>
+      <c r="E264" s="12">
+        <v>0</v>
+      </c>
+      <c r="F264">
+        <v>8</v>
+      </c>
+      <c r="G264">
+        <v>2</v>
+      </c>
+      <c r="H264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A265" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B265" s="11">
+        <v>14</v>
+      </c>
+      <c r="C265" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D265" s="12">
+        <v>4</v>
+      </c>
+      <c r="E265" s="12">
+        <v>0</v>
+      </c>
+      <c r="F265">
+        <v>3</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+      <c r="H265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A266" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B266" s="11">
+        <v>14</v>
+      </c>
+      <c r="C266" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D266" s="12">
+        <v>6</v>
+      </c>
+      <c r="E266" s="12">
+        <v>0</v>
+      </c>
+      <c r="F266">
+        <v>5</v>
+      </c>
+      <c r="G266">
+        <v>1</v>
+      </c>
+      <c r="H266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A267" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B267" s="11">
+        <v>14</v>
+      </c>
+      <c r="C267" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D267" s="12">
+        <v>1</v>
+      </c>
+      <c r="E267" s="12">
+        <v>0</v>
+      </c>
+      <c r="F267">
+        <v>1</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A268" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B268" s="11">
+        <v>14</v>
+      </c>
+      <c r="C268" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D268" s="12">
+        <v>10</v>
+      </c>
+      <c r="E268" s="12">
+        <v>0</v>
+      </c>
+      <c r="F268">
+        <v>2</v>
+      </c>
+      <c r="G268">
+        <v>8</v>
+      </c>
+      <c r="H268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A269" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B269" s="11">
+        <v>14</v>
+      </c>
+      <c r="C269" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D269" s="12">
+        <v>2</v>
+      </c>
+      <c r="E269" s="12">
+        <v>0</v>
+      </c>
+      <c r="F269">
+        <v>2</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A270" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B270" s="11">
+        <v>14</v>
+      </c>
+      <c r="C270" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D270" s="12">
+        <v>2</v>
+      </c>
+      <c r="E270" s="12">
+        <v>0</v>
+      </c>
+      <c r="F270">
+        <v>2</v>
+      </c>
+      <c r="G270">
+        <v>0</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A271" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B271" s="11">
+        <v>14</v>
+      </c>
+      <c r="C271" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D271" s="12">
+        <v>1</v>
+      </c>
+      <c r="E271" s="12">
+        <v>0</v>
+      </c>
+      <c r="F271">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
+      <c r="H271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A272" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B272" s="11">
+        <v>14</v>
+      </c>
+      <c r="C272" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D272" s="12">
+        <v>1</v>
+      </c>
+      <c r="E272" s="12">
+        <v>0</v>
+      </c>
+      <c r="F272">
+        <v>1</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+      <c r="H272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A273" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B273" s="11">
+        <v>14</v>
+      </c>
+      <c r="C273" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D273" s="12">
+        <v>2</v>
+      </c>
+      <c r="E273" s="12">
+        <v>0</v>
+      </c>
+      <c r="F273">
+        <v>1</v>
+      </c>
+      <c r="G273">
+        <v>1</v>
+      </c>
+      <c r="H273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A274" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B274" s="11">
+        <v>14</v>
+      </c>
+      <c r="C274" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D274" s="12">
+        <v>5</v>
+      </c>
+      <c r="E274" s="12">
+        <v>0</v>
+      </c>
+      <c r="F274">
+        <v>5</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+      <c r="H274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A275" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B275" s="11">
+        <v>14</v>
+      </c>
+      <c r="C275" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D275" s="13">
+        <v>15</v>
+      </c>
+      <c r="E275" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A276" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B276" s="11">
+        <v>14</v>
+      </c>
+      <c r="C276" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D276" s="13">
+        <v>8</v>
+      </c>
+      <c r="E276" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A277" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B277" s="11">
+        <v>14</v>
+      </c>
+      <c r="C277" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D277" s="13">
+        <v>10</v>
+      </c>
+      <c r="E277" s="13">
         <v>0</v>
       </c>
     </row>
@@ -5786,10 +6472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790E6A4C-D365-9744-96B0-CEA155AE8B0E}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -6805,6 +7491,160 @@
         <v>51</v>
       </c>
       <c r="D72" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A73" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D73" s="15">
+        <v>17391</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A74" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="15">
+        <v>17238</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A75" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A76" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="15">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A77" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="15">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A78" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" s="15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A79" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A80" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A81" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A82" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A83" s="14">
+        <v>43864</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="15" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Who Situation Report 15 & 16 data updated
</commit_message>
<xml_diff>
--- a/who-confirmed-cases.xlsx
+++ b/who-confirmed-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mink/Documents/GitHub/2019-nCoV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C0E877F-1934-6947-9E25-4822C7CD0AE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3DAC97-0C95-664B-9726-EF779E5EA438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WHO-Data" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="76">
   <si>
     <t>China</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Transmission Site under investigation</t>
+  </si>
+  <si>
+    <t>Belgium</t>
   </si>
 </sst>
 </file>
@@ -1540,20 +1543,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8641C3A-DA45-1B41-BC10-1E7E8EC457C5}">
-  <dimension ref="A1:H277"/>
+  <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H275" sqref="H275"/>
+      <selection pane="bottomLeft" activeCell="G329" sqref="G329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="9"/>
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="70" x14ac:dyDescent="0.15">
@@ -6462,6 +6467,1361 @@
         <v>10</v>
       </c>
       <c r="E277" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A278" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B278" s="11">
+        <v>15</v>
+      </c>
+      <c r="C278" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D278" s="12">
+        <v>20471</v>
+      </c>
+      <c r="E278" s="12">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A279" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B279" s="11">
+        <v>15</v>
+      </c>
+      <c r="C279" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D279" s="12">
+        <v>20</v>
+      </c>
+      <c r="E279" s="12">
+        <v>0</v>
+      </c>
+      <c r="F279">
+        <v>17</v>
+      </c>
+      <c r="G279">
+        <v>3</v>
+      </c>
+      <c r="H279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A280" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B280" s="11">
+        <v>15</v>
+      </c>
+      <c r="C280" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D280" s="12">
+        <v>16</v>
+      </c>
+      <c r="E280" s="12">
+        <v>0</v>
+      </c>
+      <c r="F280">
+        <v>8</v>
+      </c>
+      <c r="G280">
+        <v>5</v>
+      </c>
+      <c r="H280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A281" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B281" s="11">
+        <v>15</v>
+      </c>
+      <c r="C281" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D281" s="12">
+        <v>9</v>
+      </c>
+      <c r="E281" s="12">
+        <v>0</v>
+      </c>
+      <c r="F281">
+        <v>7</v>
+      </c>
+      <c r="G281">
+        <v>2</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A282" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B282" s="11">
+        <v>15</v>
+      </c>
+      <c r="C282" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D282" s="12">
+        <v>18</v>
+      </c>
+      <c r="E282" s="12">
+        <v>0</v>
+      </c>
+      <c r="F282">
+        <v>18</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A283" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B283" s="11">
+        <v>15</v>
+      </c>
+      <c r="C283" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D283" s="12">
+        <v>12</v>
+      </c>
+      <c r="E283" s="12">
+        <v>0</v>
+      </c>
+      <c r="F283">
+        <v>12</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+      <c r="H283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A284" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B284" s="11">
+        <v>15</v>
+      </c>
+      <c r="C284" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D284" s="12">
+        <v>10</v>
+      </c>
+      <c r="E284" s="12">
+        <v>0</v>
+      </c>
+      <c r="F284">
+        <v>7</v>
+      </c>
+      <c r="G284">
+        <v>3</v>
+      </c>
+      <c r="H284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A285" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B285" s="11">
+        <v>15</v>
+      </c>
+      <c r="C285" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D285" s="12">
+        <v>1</v>
+      </c>
+      <c r="E285" s="12">
+        <v>0</v>
+      </c>
+      <c r="F285">
+        <v>1</v>
+      </c>
+      <c r="G285">
+        <v>0</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A286" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B286" s="11">
+        <v>15</v>
+      </c>
+      <c r="C286" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D286" s="12">
+        <v>2</v>
+      </c>
+      <c r="E286" s="12">
+        <v>1</v>
+      </c>
+      <c r="F286">
+        <v>1</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
+      <c r="H286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A287" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B287" s="11">
+        <v>15</v>
+      </c>
+      <c r="C287" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D287" s="12">
+        <v>19</v>
+      </c>
+      <c r="E287" s="12">
+        <v>0</v>
+      </c>
+      <c r="F287">
+        <v>18</v>
+      </c>
+      <c r="G287">
+        <v>1</v>
+      </c>
+      <c r="H287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A288" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B288" s="11">
+        <v>15</v>
+      </c>
+      <c r="C288" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D288" s="12">
+        <v>1</v>
+      </c>
+      <c r="E288" s="12">
+        <v>0</v>
+      </c>
+      <c r="F288">
+        <v>1</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A289" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B289" s="11">
+        <v>15</v>
+      </c>
+      <c r="C289" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D289" s="12">
+        <v>1</v>
+      </c>
+      <c r="E289" s="12">
+        <v>0</v>
+      </c>
+      <c r="F289">
+        <v>1</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+      <c r="H289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A290" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B290" s="11">
+        <v>15</v>
+      </c>
+      <c r="C290" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D290" s="12">
+        <v>3</v>
+      </c>
+      <c r="E290" s="12">
+        <v>0</v>
+      </c>
+      <c r="F290">
+        <v>3</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A291" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B291" s="11">
+        <v>15</v>
+      </c>
+      <c r="C291" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D291" s="12">
+        <v>11</v>
+      </c>
+      <c r="E291" s="12">
+        <v>0</v>
+      </c>
+      <c r="F291">
+        <v>8</v>
+      </c>
+      <c r="G291">
+        <v>2</v>
+      </c>
+      <c r="H291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A292" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B292" s="11">
+        <v>15</v>
+      </c>
+      <c r="C292" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D292" s="12">
+        <v>4</v>
+      </c>
+      <c r="E292" s="12">
+        <v>0</v>
+      </c>
+      <c r="F292">
+        <v>3</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+      <c r="H292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A293" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B293" s="11">
+        <v>15</v>
+      </c>
+      <c r="C293" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D293" s="12">
+        <v>6</v>
+      </c>
+      <c r="E293" s="12">
+        <v>0</v>
+      </c>
+      <c r="F293">
+        <v>5</v>
+      </c>
+      <c r="G293">
+        <v>1</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A294" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B294" s="11">
+        <v>15</v>
+      </c>
+      <c r="C294" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D294" s="12">
+        <v>1</v>
+      </c>
+      <c r="E294" s="12">
+        <v>0</v>
+      </c>
+      <c r="F294">
+        <v>1</v>
+      </c>
+      <c r="G294">
+        <v>0</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A295" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B295" s="11">
+        <v>15</v>
+      </c>
+      <c r="C295" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D295" s="12">
+        <v>12</v>
+      </c>
+      <c r="E295" s="12">
+        <v>0</v>
+      </c>
+      <c r="F295">
+        <v>2</v>
+      </c>
+      <c r="G295">
+        <v>10</v>
+      </c>
+      <c r="H295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A296" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B296" s="11">
+        <v>15</v>
+      </c>
+      <c r="C296" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D296" s="12">
+        <v>2</v>
+      </c>
+      <c r="E296" s="12">
+        <v>0</v>
+      </c>
+      <c r="F296">
+        <v>2</v>
+      </c>
+      <c r="G296">
+        <v>0</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A297" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B297" s="11">
+        <v>15</v>
+      </c>
+      <c r="C297" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D297" s="12">
+        <v>2</v>
+      </c>
+      <c r="E297" s="12">
+        <v>0</v>
+      </c>
+      <c r="F297">
+        <v>2</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+      <c r="H297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A298" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B298" s="11">
+        <v>15</v>
+      </c>
+      <c r="C298" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D298" s="12">
+        <v>1</v>
+      </c>
+      <c r="E298" s="12">
+        <v>0</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
+      </c>
+      <c r="G298">
+        <v>1</v>
+      </c>
+      <c r="H298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A299" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B299" s="11">
+        <v>15</v>
+      </c>
+      <c r="C299" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D299" s="12">
+        <v>1</v>
+      </c>
+      <c r="E299" s="12">
+        <v>0</v>
+      </c>
+      <c r="F299">
+        <v>1</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+      <c r="H299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A300" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B300" s="11">
+        <v>15</v>
+      </c>
+      <c r="C300" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D300" s="12">
+        <v>2</v>
+      </c>
+      <c r="E300" s="12">
+        <v>0</v>
+      </c>
+      <c r="F300">
+        <v>1</v>
+      </c>
+      <c r="G300">
+        <v>1</v>
+      </c>
+      <c r="H300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A301" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B301" s="11">
+        <v>15</v>
+      </c>
+      <c r="C301" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D301" s="12">
+        <v>5</v>
+      </c>
+      <c r="E301" s="12">
+        <v>0</v>
+      </c>
+      <c r="F301">
+        <v>5</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+      <c r="H301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A302" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B302" s="11">
+        <v>15</v>
+      </c>
+      <c r="C302" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D302" s="13">
+        <v>15</v>
+      </c>
+      <c r="E302" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A303" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B303" s="11">
+        <v>15</v>
+      </c>
+      <c r="C303" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D303" s="13">
+        <v>8</v>
+      </c>
+      <c r="E303" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A304" s="10">
+        <v>43865</v>
+      </c>
+      <c r="B304" s="11">
+        <v>15</v>
+      </c>
+      <c r="C304" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D304" s="13">
+        <v>10</v>
+      </c>
+      <c r="E304" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A305" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B305" s="11">
+        <v>16</v>
+      </c>
+      <c r="C305" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D305" s="12">
+        <v>24363</v>
+      </c>
+      <c r="E305" s="12">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A306" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B306" s="11">
+        <v>16</v>
+      </c>
+      <c r="C306" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D306" s="12">
+        <v>33</v>
+      </c>
+      <c r="E306" s="12">
+        <v>0</v>
+      </c>
+      <c r="F306">
+        <v>20</v>
+      </c>
+      <c r="G306">
+        <v>13</v>
+      </c>
+      <c r="H306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A307" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B307" s="11">
+        <v>16</v>
+      </c>
+      <c r="C307" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D307" s="12">
+        <v>18</v>
+      </c>
+      <c r="E307" s="12">
+        <v>0</v>
+      </c>
+      <c r="F307">
+        <v>8</v>
+      </c>
+      <c r="G307">
+        <v>7</v>
+      </c>
+      <c r="H307">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A308" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B308" s="11">
+        <v>16</v>
+      </c>
+      <c r="C308" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D308" s="12">
+        <v>10</v>
+      </c>
+      <c r="E308" s="12">
+        <v>0</v>
+      </c>
+      <c r="F308">
+        <v>6</v>
+      </c>
+      <c r="G308">
+        <v>3</v>
+      </c>
+      <c r="H308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A309" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B309" s="11">
+        <v>16</v>
+      </c>
+      <c r="C309" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D309" s="12">
+        <v>24</v>
+      </c>
+      <c r="E309" s="12">
+        <v>0</v>
+      </c>
+      <c r="F309">
+        <v>20</v>
+      </c>
+      <c r="G309">
+        <v>4</v>
+      </c>
+      <c r="H309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A310" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B310" s="11">
+        <v>16</v>
+      </c>
+      <c r="C310" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D310" s="12">
+        <v>13</v>
+      </c>
+      <c r="E310" s="12">
+        <v>0</v>
+      </c>
+      <c r="F310">
+        <v>13</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A311" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B311" s="11">
+        <v>16</v>
+      </c>
+      <c r="C311" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D311" s="12">
+        <v>10</v>
+      </c>
+      <c r="E311" s="12">
+        <v>0</v>
+      </c>
+      <c r="F311">
+        <v>7</v>
+      </c>
+      <c r="G311">
+        <v>2</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A312" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B312" s="11">
+        <v>16</v>
+      </c>
+      <c r="C312" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D312" s="12">
+        <v>1</v>
+      </c>
+      <c r="E312" s="12">
+        <v>0</v>
+      </c>
+      <c r="F312">
+        <v>1</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A313" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B313" s="11">
+        <v>16</v>
+      </c>
+      <c r="C313" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D313" s="12">
+        <v>3</v>
+      </c>
+      <c r="E313" s="12">
+        <v>1</v>
+      </c>
+      <c r="F313">
+        <v>2</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+      <c r="H313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A314" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B314" s="11">
+        <v>16</v>
+      </c>
+      <c r="C314" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D314" s="12">
+        <v>25</v>
+      </c>
+      <c r="E314" s="12">
+        <v>0</v>
+      </c>
+      <c r="F314">
+        <v>20</v>
+      </c>
+      <c r="G314">
+        <v>5</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A315" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B315" s="11">
+        <v>16</v>
+      </c>
+      <c r="C315" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D315" s="12">
+        <v>1</v>
+      </c>
+      <c r="E315" s="12">
+        <v>0</v>
+      </c>
+      <c r="F315">
+        <v>1</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A316" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B316" s="11">
+        <v>16</v>
+      </c>
+      <c r="C316" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D316" s="12">
+        <v>1</v>
+      </c>
+      <c r="E316" s="12">
+        <v>0</v>
+      </c>
+      <c r="F316">
+        <v>1</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A317" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B317" s="11">
+        <v>16</v>
+      </c>
+      <c r="C317" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D317" s="12">
+        <v>3</v>
+      </c>
+      <c r="E317" s="12">
+        <v>0</v>
+      </c>
+      <c r="F317">
+        <v>3</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A318" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B318" s="11">
+        <v>16</v>
+      </c>
+      <c r="C318" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D318" s="12">
+        <v>11</v>
+      </c>
+      <c r="E318" s="12">
+        <v>0</v>
+      </c>
+      <c r="F318">
+        <v>8</v>
+      </c>
+      <c r="G318">
+        <v>2</v>
+      </c>
+      <c r="H318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A319" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B319" s="11">
+        <v>16</v>
+      </c>
+      <c r="C319" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D319" s="12">
+        <v>5</v>
+      </c>
+      <c r="E319" s="12">
+        <v>0</v>
+      </c>
+      <c r="F319">
+        <v>3</v>
+      </c>
+      <c r="G319">
+        <v>1</v>
+      </c>
+      <c r="H319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A320" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B320" s="11">
+        <v>16</v>
+      </c>
+      <c r="C320" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D320" s="12">
+        <v>6</v>
+      </c>
+      <c r="E320" s="12">
+        <v>0</v>
+      </c>
+      <c r="F320">
+        <v>5</v>
+      </c>
+      <c r="G320">
+        <v>1</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A321" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B321" s="11">
+        <v>16</v>
+      </c>
+      <c r="C321" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D321" s="12">
+        <v>1</v>
+      </c>
+      <c r="E321" s="12">
+        <v>0</v>
+      </c>
+      <c r="F321">
+        <v>1</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+      <c r="H321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A322" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B322" s="11">
+        <v>16</v>
+      </c>
+      <c r="C322" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D322" s="12">
+        <v>12</v>
+      </c>
+      <c r="E322" s="12">
+        <v>0</v>
+      </c>
+      <c r="F322">
+        <v>2</v>
+      </c>
+      <c r="G322">
+        <v>10</v>
+      </c>
+      <c r="H322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A323" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B323" s="11">
+        <v>16</v>
+      </c>
+      <c r="C323" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D323" s="12">
+        <v>2</v>
+      </c>
+      <c r="E323" s="12">
+        <v>0</v>
+      </c>
+      <c r="F323">
+        <v>2</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+      <c r="H323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A324" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B324" s="11">
+        <v>16</v>
+      </c>
+      <c r="C324" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D324" s="12">
+        <v>2</v>
+      </c>
+      <c r="E324" s="12">
+        <v>0</v>
+      </c>
+      <c r="F324">
+        <v>2</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+      <c r="H324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A325" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B325" s="11">
+        <v>16</v>
+      </c>
+      <c r="C325" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D325" s="12">
+        <v>1</v>
+      </c>
+      <c r="E325" s="12">
+        <v>0</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+      <c r="G325">
+        <v>1</v>
+      </c>
+      <c r="H325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A326" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B326" s="11">
+        <v>16</v>
+      </c>
+      <c r="C326" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D326" s="12">
+        <v>1</v>
+      </c>
+      <c r="E326" s="12">
+        <v>0</v>
+      </c>
+      <c r="F326">
+        <v>1</v>
+      </c>
+      <c r="G326">
+        <v>0</v>
+      </c>
+      <c r="H326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A327" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B327" s="11">
+        <v>16</v>
+      </c>
+      <c r="C327" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D327" s="12">
+        <v>2</v>
+      </c>
+      <c r="E327" s="12">
+        <v>0</v>
+      </c>
+      <c r="F327">
+        <v>1</v>
+      </c>
+      <c r="G327">
+        <v>1</v>
+      </c>
+      <c r="H327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A328" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B328" s="11">
+        <v>16</v>
+      </c>
+      <c r="C328" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D328" s="12">
+        <v>1</v>
+      </c>
+      <c r="E328" s="12">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <v>1</v>
+      </c>
+      <c r="G328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" ht="17" x14ac:dyDescent="0.15">
+      <c r="A329" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B329" s="11">
+        <v>16</v>
+      </c>
+      <c r="C329" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D329" s="12">
+        <v>5</v>
+      </c>
+      <c r="E329" s="12">
+        <v>0</v>
+      </c>
+      <c r="F329">
+        <v>5</v>
+      </c>
+      <c r="G329">
+        <v>0</v>
+      </c>
+      <c r="H329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A330" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B330" s="11">
+        <v>16</v>
+      </c>
+      <c r="C330" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D330" s="13">
+        <v>15</v>
+      </c>
+      <c r="E330" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A331" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B331" s="11">
+        <v>16</v>
+      </c>
+      <c r="C331" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D331" s="13">
+        <v>8</v>
+      </c>
+      <c r="E331" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A332" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B332" s="11">
+        <v>16</v>
+      </c>
+      <c r="C332" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D332" s="13">
+        <v>10</v>
+      </c>
+      <c r="E332" s="13">
         <v>0</v>
       </c>
     </row>
@@ -6472,10 +7832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790E6A4C-D365-9744-96B0-CEA155AE8B0E}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A73" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -7648,6 +9008,314 @@
         <v>53</v>
       </c>
     </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A84" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" s="15">
+        <v>20630</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A85" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D85" s="15">
+        <v>20471</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A86" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A87" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="15">
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A88" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="15">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A89" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D89" s="15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A90" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A91" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A92" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A93" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A94" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A95" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D95" s="15">
+        <v>24554</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A96" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D96" s="15">
+        <v>24363</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A97" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A98" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="15">
+        <v>3219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A99" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="15">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A100" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D100" s="15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A101" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A102" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A103" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A104" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A105" s="14">
+        <v>43866</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7657,7 +9325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EF8EEC-06D7-D247-8015-084E719ED0B9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sit Rep 15 & 16 update
</commit_message>
<xml_diff>
--- a/who-confirmed-cases.xlsx
+++ b/who-confirmed-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mink/Documents/GitHub/2019-nCoV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3DAC97-0C95-664B-9726-EF779E5EA438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11AEA34-91DB-FE4C-A140-44E8A4D100C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WHO-Data" sheetId="2" r:id="rId1"/>
@@ -1545,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8641C3A-DA45-1B41-BC10-1E7E8EC457C5}">
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="G329" sqref="G329"/>
@@ -9325,7 +9325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EF8EEC-06D7-D247-8015-084E719ED0B9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Errata published re canada
</commit_message>
<xml_diff>
--- a/who-confirmed-cases.xlsx
+++ b/who-confirmed-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mink/Documents/GitHub/2019-nCoV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11AEA34-91DB-FE4C-A140-44E8A4D100C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401050DE-4C30-3040-A574-6F982D334BCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19040" yWindow="2260" windowWidth="19020" windowHeight="24060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1546,9 +1546,9 @@
   <dimension ref="A1:H332"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G329" sqref="G329"/>
+      <selection pane="bottomLeft" activeCell="F320" sqref="F320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1561,7 +1561,7 @@
     <col min="7" max="7" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="98" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -7505,10 +7505,10 @@
         <v>5</v>
       </c>
       <c r="E319" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F319">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G319">
         <v>1</v>

</xml_diff>